<commit_message>
more progress on parsing
</commit_message>
<xml_diff>
--- a/valid mode bit table.xlsx
+++ b/valid mode bit table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cam\Documents\CSS\422\Final project\Asm-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F670217-B2FA-4D7A-B079-1F828BEFD520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5243AD8-4BED-4BD6-99B1-EF3D07C28F47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12840" yWindow="2028" windowWidth="9648" windowHeight="8964" xr2:uid="{22575524-D629-4AB5-9811-2576EA4A51CC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>MOVE</t>
   </si>
@@ -146,10 +146,10 @@
     <t>0x19D</t>
   </si>
   <si>
-    <t>0x19C</t>
-  </si>
-  <si>
-    <t>0x1</t>
+    <t>LSd</t>
+  </si>
+  <si>
+    <t>ASd</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:M25"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -687,492 +687,168 @@
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5" t="s">
-        <v>37</v>
-      </c>
-      <c r="O5" t="str">
-        <f t="shared" si="0"/>
-        <v>19D</v>
-      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O6" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7" t="s">
-        <v>37</v>
-      </c>
-      <c r="O7" t="str">
-        <f t="shared" si="0"/>
-        <v>19D</v>
-      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="N8" t="s">
-        <v>38</v>
-      </c>
-      <c r="O8" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
-        <v>1</v>
-      </c>
-      <c r="N9" t="s">
-        <v>37</v>
-      </c>
-      <c r="O9" t="str">
-        <f t="shared" si="0"/>
-        <v>19D</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N10" t="s">
-        <v>38</v>
-      </c>
-      <c r="O10" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>1</v>
-      </c>
-      <c r="N11" t="s">
-        <v>38</v>
-      </c>
-      <c r="O11" t="str">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
-        <v>1</v>
-      </c>
-      <c r="N12" t="s">
-        <v>38</v>
-      </c>
-      <c r="O12" t="str">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>1</v>
-      </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>1</v>
-      </c>
-      <c r="N13" t="s">
-        <v>36</v>
-      </c>
-      <c r="O13" t="str">
-        <f t="shared" si="0"/>
-        <v>19D</v>
-      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="N14" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="N16" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="N17" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" t="str">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="M21" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>36</v>
+      </c>
+      <c r="O21" t="str">
+        <f>DEC2HEX(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(_xlfn.BITLSHIFT(B21,1)+C21,1)+D21,1)+E21,1)+F21,1)+G21,1)+H21,1)+I21,1)+J21,1)+K21,1)+L21,1)+M21)</f>
+        <v>19D</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1284,6 +960,12 @@
       <c r="D24">
         <v>0</v>
       </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
       <c r="G24">
         <v>0</v>
       </c>
@@ -1291,20 +973,26 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
       </c>
       <c r="L24">
         <v>0</v>
+      </c>
+      <c r="M24">
+        <v>1</v>
       </c>
       <c r="N24" t="s">
         <v>33</v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19D</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -1320,10 +1008,31 @@
       <c r="D25">
         <v>0</v>
       </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
         <v>0</v>
       </c>
       <c r="N25" t="s">
@@ -1331,7 +1040,7 @@
       </c>
       <c r="O25" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19C</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -1347,18 +1056,39 @@
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>1</v>
       </c>
       <c r="N26" t="s">
         <v>33</v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19D</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
@@ -1374,10 +1104,31 @@
       <c r="D27">
         <v>0</v>
       </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
         <v>0</v>
       </c>
       <c r="N27" t="s">
@@ -1385,7 +1136,7 @@
       </c>
       <c r="O27" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19C</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
@@ -1401,18 +1152,39 @@
       <c r="D28">
         <v>0</v>
       </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
       <c r="G28">
         <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>1</v>
       </c>
       <c r="N28" t="s">
         <v>33</v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19D</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -1428,10 +1200,31 @@
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
       <c r="G29">
         <v>0</v>
       </c>
       <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
         <v>0</v>
       </c>
       <c r="N29" t="s">
@@ -1439,7 +1232,7 @@
       </c>
       <c r="O29" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>19C</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1455,18 +1248,36 @@
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
       <c r="G30">
         <v>0</v>
       </c>
       <c r="H30">
         <v>0</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <v>1</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
       </c>
       <c r="N30" t="s">
         <v>33</v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>99D</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -1482,18 +1293,36 @@
       <c r="D31">
         <v>0</v>
       </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
       <c r="G31">
         <v>0</v>
       </c>
       <c r="H31">
         <v>0</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
       </c>
       <c r="N31" t="s">
         <v>33</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="1"/>
-        <v>800</v>
+        <v>99D</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -1537,7 +1366,10 @@
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
       </c>
       <c r="C33">
         <v>0</v>
@@ -1545,23 +1377,26 @@
       <c r="D33">
         <v>0</v>
       </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-      <c r="H33">
-        <v>0</v>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
       </c>
       <c r="N33" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
       </c>
       <c r="C34">
         <v>0</v>
@@ -1569,18 +1404,18 @@
       <c r="D34">
         <v>0</v>
       </c>
-      <c r="G34">
-        <v>0</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
       </c>
       <c r="N34" t="s">
         <v>33</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>